<commit_message>
LSTM multivariate model Finalized
- save all the plots, models, prediction
</commit_message>
<xml_diff>
--- a/France_sweet_spot.xlsx
+++ b/France_sweet_spot.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rezan\Documents\Master in Applied Data Science\2nd Year\MASTER THESIS\GIT THESIS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D7DF669-4043-411D-A179-395654D0041B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A9F0585-40ED-45CC-B2EE-BB2E60FFF854}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="666" uniqueCount="337">
   <si>
     <t>region_found</t>
   </si>
@@ -595,30 +595,15 @@
     <t>RMSE_train</t>
   </si>
   <si>
-    <t>model_name</t>
-  </si>
-  <si>
-    <t>best_model_uni.h5</t>
-  </si>
-  <si>
     <t>2.24</t>
   </si>
   <si>
     <t>RMSE_valid</t>
   </si>
   <si>
-    <t xml:space="preserve">2.02 </t>
-  </si>
-  <si>
     <t>model evaluation</t>
   </si>
   <si>
-    <t>0.0032788857351988554</t>
-  </si>
-  <si>
-    <t>0.012085831724107265</t>
-  </si>
-  <si>
     <t>Anjou.h5</t>
   </si>
   <si>
@@ -628,25 +613,16 @@
     <t>Beaujolais.h5</t>
   </si>
   <si>
-    <t>Beaujolais Blanc.h5</t>
-  </si>
-  <si>
     <t>2.07</t>
   </si>
   <si>
     <t>2.14</t>
   </si>
   <si>
-    <t xml:space="preserve">1.51 </t>
-  </si>
-  <si>
-    <t>1.45</t>
-  </si>
-  <si>
-    <t>0.008383103646337986</t>
-  </si>
-  <si>
-    <t>0.0031919809989631176</t>
+    <t>1.97</t>
+  </si>
+  <si>
+    <t>1.89</t>
   </si>
   <si>
     <t>1.73</t>
@@ -655,20 +631,416 @@
     <t>1.90</t>
   </si>
   <si>
-    <t>2.0</t>
-  </si>
-  <si>
-    <t>2.15</t>
-  </si>
-  <si>
-    <t>0.005191273987293243</t>
+    <t>Alsace.h5</t>
+  </si>
+  <si>
+    <t>2.23</t>
+  </si>
+  <si>
+    <t>0.0027467464096844196</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.15 </t>
+  </si>
+  <si>
+    <t>2.05</t>
+  </si>
+  <si>
+    <t>2.22</t>
+  </si>
+  <si>
+    <t>0.0002934987423941493</t>
+  </si>
+  <si>
+    <t>1.46</t>
+  </si>
+  <si>
+    <t>1.74</t>
+  </si>
+  <si>
+    <t>1.61</t>
+  </si>
+  <si>
+    <t>0.013371596112847328</t>
+  </si>
+  <si>
+    <t>1.62</t>
+  </si>
+  <si>
+    <t>1.92</t>
+  </si>
+  <si>
+    <t>0.0023579788394272327</t>
+  </si>
+  <si>
+    <t>2.01</t>
+  </si>
+  <si>
+    <t>2.17</t>
+  </si>
+  <si>
+    <t>model_name (region_name.h5)</t>
+  </si>
+  <si>
+    <t>0.004762586206197739</t>
+  </si>
+  <si>
+    <t>2.00</t>
+  </si>
+  <si>
+    <t>2.20</t>
+  </si>
+  <si>
+    <t>0.003740040585398674</t>
+  </si>
+  <si>
+    <t>1.91</t>
+  </si>
+  <si>
+    <t>2.18</t>
+  </si>
+  <si>
+    <t>0.0006676570628769696</t>
+  </si>
+  <si>
+    <t>1.81</t>
+  </si>
+  <si>
+    <t>0.0035557840019464493</t>
+  </si>
+  <si>
+    <t>2.09</t>
+  </si>
+  <si>
+    <t>1.99</t>
+  </si>
+  <si>
+    <t>1.88</t>
+  </si>
+  <si>
+    <t>0.005178520921617746</t>
+  </si>
+  <si>
+    <t>1.86</t>
+  </si>
+  <si>
+    <t>1.83</t>
+  </si>
+  <si>
+    <t>0.0020468260627239943</t>
+  </si>
+  <si>
+    <t>1.96</t>
+  </si>
+  <si>
+    <t>2.38</t>
+  </si>
+  <si>
+    <t>1.93</t>
+  </si>
+  <si>
+    <t>2.35</t>
+  </si>
+  <si>
+    <t>0.00010986885172314942</t>
+  </si>
+  <si>
+    <t>1.19</t>
+  </si>
+  <si>
+    <t>1.27</t>
+  </si>
+  <si>
+    <t>0.0022584092803299427</t>
+  </si>
+  <si>
+    <t>1.82</t>
+  </si>
+  <si>
+    <t>1.98</t>
+  </si>
+  <si>
+    <t>0.0030729700811207294</t>
+  </si>
+  <si>
+    <t>1.78</t>
+  </si>
+  <si>
+    <t>2.13</t>
+  </si>
+  <si>
+    <t>0.003603180404752493</t>
+  </si>
+  <si>
+    <t>1.79</t>
+  </si>
+  <si>
+    <t>1.94</t>
+  </si>
+  <si>
+    <t>2.10</t>
+  </si>
+  <si>
+    <t>0.0036137248389422894</t>
+  </si>
+  <si>
+    <t>0.0035716535057872534</t>
+  </si>
+  <si>
+    <t>0.00453437864780426</t>
+  </si>
+  <si>
+    <t>2.41</t>
+  </si>
+  <si>
+    <t>0.0025465404614806175</t>
+  </si>
+  <si>
+    <t>0.004847971256822348</t>
+  </si>
+  <si>
+    <t>1.71</t>
+  </si>
+  <si>
+    <t>1.84</t>
+  </si>
+  <si>
+    <t>2.02</t>
+  </si>
+  <si>
+    <t>2.12</t>
+  </si>
+  <si>
+    <t>0.00418079411610961</t>
+  </si>
+  <si>
+    <t>1.72</t>
+  </si>
+  <si>
+    <t>0.00012674002209678292</t>
+  </si>
+  <si>
+    <t>2.03</t>
+  </si>
+  <si>
+    <t>0.0029927080031484365</t>
+  </si>
+  <si>
+    <t>1.77</t>
+  </si>
+  <si>
+    <t>0.0038093195762485266</t>
+  </si>
+  <si>
+    <t>1.75</t>
+  </si>
+  <si>
+    <t>0.003825305961072445</t>
+  </si>
+  <si>
+    <t>2.21</t>
+  </si>
+  <si>
+    <t>0.002415964612737298</t>
+  </si>
+  <si>
+    <t>2.04</t>
+  </si>
+  <si>
+    <t>0.003947296179831028</t>
+  </si>
+  <si>
+    <t>1.64</t>
+  </si>
+  <si>
+    <t>1.57</t>
+  </si>
+  <si>
+    <t>2.27</t>
+  </si>
+  <si>
+    <t>1.30</t>
+  </si>
+  <si>
+    <t>0.0038864752277731895</t>
+  </si>
+  <si>
+    <t>0.004746128339320421</t>
+  </si>
+  <si>
+    <t>0.0034866167698055506</t>
+  </si>
+  <si>
+    <t>0.0004391580878291279</t>
+  </si>
+  <si>
+    <t>2.16</t>
+  </si>
+  <si>
+    <t>0.0044731879606842995</t>
+  </si>
+  <si>
+    <t>0.004292540717869997</t>
+  </si>
+  <si>
+    <t>1.60</t>
+  </si>
+  <si>
+    <t>0.0038289306685328484</t>
+  </si>
+  <si>
+    <t>2.26</t>
+  </si>
+  <si>
+    <t>0.003929227590560913</t>
+  </si>
+  <si>
+    <t>2.30</t>
+  </si>
+  <si>
+    <t>0.0021771006286144257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.98 </t>
+  </si>
+  <si>
+    <t>2.19</t>
+  </si>
+  <si>
+    <t>0.0028868436347693205</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.86 </t>
+  </si>
+  <si>
+    <t>0.006665917579084635</t>
+  </si>
+  <si>
+    <t>0.00019793902174569666</t>
+  </si>
+  <si>
+    <t>0.003973100800067186</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1.92 </t>
+  </si>
+  <si>
+    <t>2.36</t>
+  </si>
+  <si>
+    <t>0.0001791087124729529</t>
+  </si>
+  <si>
+    <t>0.35</t>
+  </si>
+  <si>
+    <t>0.42</t>
+  </si>
+  <si>
+    <t>0.0008624259498901665</t>
+  </si>
+  <si>
+    <t>0.004047902766615152</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2.40 </t>
+  </si>
+  <si>
+    <t>0.0028562769293785095</t>
+  </si>
+  <si>
+    <t>0.0035878904163837433</t>
+  </si>
+  <si>
+    <t>2.06</t>
+  </si>
+  <si>
+    <t>0.004667527507990599</t>
+  </si>
+  <si>
+    <t>0.005129713099449873</t>
+  </si>
+  <si>
+    <t>0.0030237387400120497</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.59 </t>
+  </si>
+  <si>
+    <t>0.0034905525390058756</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.97 </t>
+  </si>
+  <si>
+    <t>2.43</t>
+  </si>
+  <si>
+    <t>0.0051896832883358</t>
+  </si>
+  <si>
+    <t>0.004106903448700905</t>
+  </si>
+  <si>
+    <t>0.005029697902500629</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1.94 </t>
+  </si>
+  <si>
+    <t>0.005000115372240543</t>
+  </si>
+  <si>
+    <t>0.0031169524881988764</t>
+  </si>
+  <si>
+    <t>2.08</t>
+  </si>
+  <si>
+    <t>0.0039672572165727615</t>
+  </si>
+  <si>
+    <t>0.0020008296705782413</t>
+  </si>
+  <si>
+    <t>0.0047006006352603436</t>
+  </si>
+  <si>
+    <t>0.004401644226163626</t>
+  </si>
+  <si>
+    <t>1.95</t>
+  </si>
+  <si>
+    <t>0.0033028670586645603</t>
+  </si>
+  <si>
+    <t>0.0005578949931077659</t>
+  </si>
+  <si>
+    <t>0.003690672107040882</t>
+  </si>
+  <si>
+    <t>1.66</t>
+  </si>
+  <si>
+    <t>0.0024261795915663242</t>
+  </si>
+  <si>
+    <t>0.0029792890418320894</t>
+  </si>
+  <si>
+    <t>1.87</t>
+  </si>
+  <si>
+    <t>0.003888244042173028</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -697,13 +1069,33 @@
       <name val="Courier New"/>
       <family val="3"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="3">
@@ -742,7 +1134,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -756,7 +1148,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1098,18 +1498,18 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:J96"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+    <sheetView tabSelected="1" topLeftCell="A84" workbookViewId="0">
+      <selection activeCell="F90" sqref="F90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="31.453125" customWidth="1"/>
-    <col min="3" max="3" width="19.26953125" customWidth="1"/>
-    <col min="6" max="6" width="30.26953125" customWidth="1"/>
+    <col min="2" max="2" width="26.6328125" customWidth="1"/>
+    <col min="3" max="3" width="23.81640625" customWidth="1"/>
+    <col min="6" max="6" width="9.453125" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="12.36328125" customWidth="1"/>
-    <col min="9" max="9" width="17.26953125" customWidth="1"/>
+    <col min="9" max="9" width="28.81640625" customWidth="1"/>
     <col min="10" max="10" width="12.6328125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1133,13 +1533,13 @@
         <v>189</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>190</v>
+        <v>218</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.35">
@@ -1162,16 +1562,16 @@
         <v>188</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="H2" s="3" t="s">
-        <v>194</v>
+        <v>206</v>
       </c>
       <c r="I2" t="s">
-        <v>191</v>
+        <v>202</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>196</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.35">
@@ -1194,16 +1594,16 @@
         <v>188</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>203</v>
+        <v>205</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>202</v>
+        <v>196</v>
       </c>
       <c r="I3" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>197</v>
+        <v>204</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.35">
@@ -1226,16 +1626,16 @@
         <v>188</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>205</v>
+        <v>211</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>204</v>
+        <v>209</v>
       </c>
       <c r="I4" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>206</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.35">
@@ -1258,16 +1658,16 @@
         <v>188</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>208</v>
+        <v>213</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>209</v>
+        <v>214</v>
       </c>
       <c r="I5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>207</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.35">
@@ -1290,16 +1690,13 @@
         <v>188</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>211</v>
+        <v>217</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="I6" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>212</v>
+        <v>219</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.35">
@@ -1318,6 +1715,18 @@
       <c r="E7" t="s">
         <v>146</v>
       </c>
+      <c r="F7" t="s">
+        <v>188</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>221</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A8" s="1">
@@ -1335,6 +1744,18 @@
       <c r="E8" t="s">
         <v>147</v>
       </c>
+      <c r="F8" t="s">
+        <v>188</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>196</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A9" s="1">
@@ -1352,6 +1773,18 @@
       <c r="E9" t="s">
         <v>148</v>
       </c>
+      <c r="F9" t="s">
+        <v>188</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>226</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>213</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="10" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1">
@@ -1403,6 +1836,18 @@
       <c r="E12" t="s">
         <v>149</v>
       </c>
+      <c r="F12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G12" s="4" t="s">
+        <v>228</v>
+      </c>
+      <c r="H12" s="4" t="s">
+        <v>223</v>
+      </c>
+      <c r="J12" s="6">
+        <v>127344065.958823</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A13" s="1">
@@ -1420,6 +1865,18 @@
       <c r="E13" t="s">
         <v>150</v>
       </c>
+      <c r="F13" t="s">
+        <v>188</v>
+      </c>
+      <c r="G13" s="4" t="s">
+        <v>230</v>
+      </c>
+      <c r="H13" s="4" t="s">
+        <v>229</v>
+      </c>
+      <c r="J13" s="3" t="s">
+        <v>231</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A14" s="1">
@@ -1437,6 +1894,18 @@
       <c r="E14" t="s">
         <v>151</v>
       </c>
+      <c r="F14" t="s">
+        <v>188</v>
+      </c>
+      <c r="G14" s="4" t="s">
+        <v>232</v>
+      </c>
+      <c r="H14" s="4" t="s">
+        <v>210</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>234</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A15" s="1">
@@ -1454,6 +1923,18 @@
       <c r="E15" t="s">
         <v>152</v>
       </c>
+      <c r="F15" t="s">
+        <v>188</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="H15" s="4" t="s">
+        <v>235</v>
+      </c>
+      <c r="J15" s="6">
+        <v>58169469411.9505</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A16" s="1">
@@ -1471,8 +1952,20 @@
       <c r="E16" t="s">
         <v>153</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F16" t="s">
+        <v>188</v>
+      </c>
+      <c r="G16" s="4" t="s">
+        <v>238</v>
+      </c>
+      <c r="H16" s="4" t="s">
+        <v>237</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1488,8 +1981,20 @@
       <c r="E17" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F17" t="s">
+        <v>188</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>217</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>240</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1506,7 +2011,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="19" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1523,7 +2028,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1539,8 +2044,20 @@
       <c r="E20" t="s">
         <v>154</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F20" t="s">
+        <v>188</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1557,7 +2074,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1574,7 +2091,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1590,8 +2107,20 @@
       <c r="E23" t="s">
         <v>155</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F23" t="s">
+        <v>188</v>
+      </c>
+      <c r="G23" t="s">
+        <v>247</v>
+      </c>
+      <c r="H23" t="s">
+        <v>246</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1607,8 +2136,20 @@
       <c r="E24" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F24" t="s">
+        <v>188</v>
+      </c>
+      <c r="G24" t="s">
+        <v>251</v>
+      </c>
+      <c r="H24" t="s">
+        <v>249</v>
+      </c>
+      <c r="J24" s="3" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1624,8 +2165,20 @@
       <c r="E25" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F25" t="s">
+        <v>188</v>
+      </c>
+      <c r="G25" t="s">
+        <v>216</v>
+      </c>
+      <c r="H25" t="s">
+        <v>244</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1641,8 +2194,20 @@
       <c r="E26" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F26" t="s">
+        <v>188</v>
+      </c>
+      <c r="G26" t="s">
+        <v>196</v>
+      </c>
+      <c r="H26" t="s">
+        <v>229</v>
+      </c>
+      <c r="J26" s="3" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1658,8 +2223,20 @@
       <c r="E27" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F27" t="s">
+        <v>188</v>
+      </c>
+      <c r="G27" t="s">
+        <v>255</v>
+      </c>
+      <c r="H27" t="s">
+        <v>233</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1675,8 +2252,20 @@
       <c r="E28" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F28" t="s">
+        <v>188</v>
+      </c>
+      <c r="G28" t="s">
+        <v>201</v>
+      </c>
+      <c r="H28" t="s">
+        <v>237</v>
+      </c>
+      <c r="J28" s="3" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1692,8 +2281,20 @@
       <c r="E29" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F29" t="s">
+        <v>188</v>
+      </c>
+      <c r="G29" t="s">
+        <v>260</v>
+      </c>
+      <c r="H29" t="s">
+        <v>232</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1709,8 +2310,20 @@
       <c r="E30" t="s">
         <v>158</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F30" t="s">
+        <v>188</v>
+      </c>
+      <c r="G30" t="s">
+        <v>263</v>
+      </c>
+      <c r="H30" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="J30" s="3" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1726,8 +2339,20 @@
       <c r="E31" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F31" t="s">
+        <v>188</v>
+      </c>
+      <c r="G31" t="s">
+        <v>265</v>
+      </c>
+      <c r="H31" t="s">
+        <v>223</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1743,8 +2368,20 @@
       <c r="E32" t="s">
         <v>159</v>
       </c>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F32" t="s">
+        <v>188</v>
+      </c>
+      <c r="G32" t="s">
+        <v>230</v>
+      </c>
+      <c r="H32" t="s">
+        <v>269</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1760,8 +2397,20 @@
       <c r="E33" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="34" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F33" t="s">
+        <v>188</v>
+      </c>
+      <c r="G33" t="s">
+        <v>203</v>
+      </c>
+      <c r="H33" t="s">
+        <v>216</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1778,7 +2427,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1794,8 +2443,20 @@
       <c r="E35" t="s">
         <v>161</v>
       </c>
-    </row>
-    <row r="36" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F35" t="s">
+        <v>188</v>
+      </c>
+      <c r="G35" t="s">
+        <v>271</v>
+      </c>
+      <c r="H35" t="s">
+        <v>210</v>
+      </c>
+      <c r="J35" s="3" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1812,7 +2473,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1828,8 +2489,20 @@
       <c r="E37" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="38" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F37" t="s">
+        <v>188</v>
+      </c>
+      <c r="G37" t="s">
+        <v>273</v>
+      </c>
+      <c r="H37" t="s">
+        <v>244</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1846,7 +2519,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1862,8 +2535,20 @@
       <c r="E39" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F39" t="s">
+        <v>188</v>
+      </c>
+      <c r="G39" t="s">
+        <v>276</v>
+      </c>
+      <c r="H39" t="s">
+        <v>275</v>
+      </c>
+      <c r="J39" s="6">
+        <v>13717128695.1343</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1879,8 +2564,20 @@
       <c r="E40" t="s">
         <v>163</v>
       </c>
-    </row>
-    <row r="41" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F40" t="s">
+        <v>188</v>
+      </c>
+      <c r="G40" t="s">
+        <v>278</v>
+      </c>
+      <c r="H40" t="s">
+        <v>241</v>
+      </c>
+      <c r="J40" s="3" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1897,7 +2594,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="42" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1914,7 +2611,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1930,8 +2627,20 @@
       <c r="E43" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F43" t="s">
+        <v>188</v>
+      </c>
+      <c r="G43" t="s">
+        <v>261</v>
+      </c>
+      <c r="H43" t="s">
+        <v>235</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1947,8 +2656,20 @@
       <c r="E44" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F44" t="s">
+        <v>188</v>
+      </c>
+      <c r="G44" t="s">
+        <v>228</v>
+      </c>
+      <c r="H44" t="s">
+        <v>233</v>
+      </c>
+      <c r="J44" s="3" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1964,8 +2685,20 @@
       <c r="E45" t="s">
         <v>165</v>
       </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F45" t="s">
+        <v>188</v>
+      </c>
+      <c r="G45" t="s">
+        <v>198</v>
+      </c>
+      <c r="H45" t="s">
+        <v>265</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1981,8 +2714,20 @@
       <c r="E46" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="47" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F46" t="s">
+        <v>188</v>
+      </c>
+      <c r="G46" t="s">
+        <v>283</v>
+      </c>
+      <c r="H46" t="s">
+        <v>216</v>
+      </c>
+      <c r="J46" s="3" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1999,7 +2744,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -2015,8 +2760,20 @@
       <c r="E48" t="s">
         <v>166</v>
       </c>
-    </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F48" t="s">
+        <v>188</v>
+      </c>
+      <c r="G48" t="s">
+        <v>198</v>
+      </c>
+      <c r="H48" t="s">
+        <v>198</v>
+      </c>
+      <c r="J48" s="3" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -2032,8 +2789,20 @@
       <c r="E49" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F49" t="s">
+        <v>188</v>
+      </c>
+      <c r="G49" t="s">
+        <v>220</v>
+      </c>
+      <c r="H49" t="s">
+        <v>201</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -2049,25 +2818,37 @@
       <c r="E50" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="1">
+      <c r="F50" t="s">
+        <v>188</v>
+      </c>
+      <c r="G50" t="s">
+        <v>190</v>
+      </c>
+      <c r="H50" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="J50" s="3" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" s="8" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="7">
         <v>49</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="9" t="s">
         <v>41</v>
       </c>
-      <c r="D51" t="s">
+      <c r="D51" s="8" t="s">
         <v>122</v>
       </c>
-      <c r="E51" t="s">
+      <c r="E51" s="8" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -2083,8 +2864,20 @@
       <c r="E52" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F52" t="s">
+        <v>188</v>
+      </c>
+      <c r="G52" t="s">
+        <v>290</v>
+      </c>
+      <c r="H52" t="s">
+        <v>214</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2100,8 +2893,20 @@
       <c r="E53" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F53" t="s">
+        <v>188</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="J53" s="3" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2117,8 +2922,20 @@
       <c r="E54" t="s">
         <v>169</v>
       </c>
-    </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F54" t="s">
+        <v>188</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="J54" s="3" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2134,8 +2951,20 @@
       <c r="E55" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F55" t="s">
+        <v>188</v>
+      </c>
+      <c r="G55" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="H55" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="J55" s="3" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2151,8 +2980,20 @@
       <c r="E56" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="57" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F56" t="s">
+        <v>188</v>
+      </c>
+      <c r="G56" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="H56" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="J56" s="3" t="s">
+        <v>298</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2169,7 +3010,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2185,8 +3026,20 @@
       <c r="E58" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F58" t="s">
+        <v>188</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2202,8 +3055,20 @@
       <c r="E59" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F59" t="s">
+        <v>188</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2219,8 +3084,20 @@
       <c r="E60" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F60" t="s">
+        <v>188</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>249</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>305</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2236,8 +3113,20 @@
       <c r="E61" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F61" t="s">
+        <v>188</v>
+      </c>
+      <c r="G61" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="H61" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="J61" s="3" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2253,8 +3142,20 @@
       <c r="E62" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F62" t="s">
+        <v>188</v>
+      </c>
+      <c r="G62" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="H62" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="J62" s="3" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2270,8 +3171,20 @@
       <c r="E63" t="s">
         <v>174</v>
       </c>
-    </row>
-    <row r="64" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F63" t="s">
+        <v>188</v>
+      </c>
+      <c r="G63" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="H63" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="J63" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2288,7 +3201,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2304,8 +3217,20 @@
       <c r="E65" t="s">
         <v>164</v>
       </c>
-    </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F65" t="s">
+        <v>188</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2321,8 +3246,20 @@
       <c r="E66" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F66" t="s">
+        <v>188</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2338,8 +3275,20 @@
       <c r="E67" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F67" t="s">
+        <v>188</v>
+      </c>
+      <c r="G67" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="H67" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="J67" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2355,8 +3304,20 @@
       <c r="E68" t="s">
         <v>175</v>
       </c>
-    </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F68" t="s">
+        <v>188</v>
+      </c>
+      <c r="G68" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="H68" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="J68" s="6">
+        <v>2403112603.1331902</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2372,8 +3333,20 @@
       <c r="E69" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F69" t="s">
+        <v>188</v>
+      </c>
+      <c r="G69" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="H69" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="J69" s="6">
+        <v>18448990886.099602</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2389,8 +3362,20 @@
       <c r="E70" t="s">
         <v>170</v>
       </c>
-    </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F70" t="s">
+        <v>188</v>
+      </c>
+      <c r="G70" s="3" t="s">
+        <v>269</v>
+      </c>
+      <c r="H70" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="J70" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2406,8 +3391,20 @@
       <c r="E71" t="s">
         <v>177</v>
       </c>
-    </row>
-    <row r="72" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F71" t="s">
+        <v>188</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="J71" s="3" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2424,7 +3421,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2440,8 +3437,20 @@
       <c r="E73" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F73" t="s">
+        <v>188</v>
+      </c>
+      <c r="G73" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="J73" s="3" t="s">
+        <v>319</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2457,8 +3466,20 @@
       <c r="E74" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F74" t="s">
+        <v>188</v>
+      </c>
+      <c r="G74" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="H74" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="J74" s="3" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2474,8 +3495,20 @@
       <c r="E75" t="s">
         <v>146</v>
       </c>
-    </row>
-    <row r="76" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+      <c r="F75" t="s">
+        <v>188</v>
+      </c>
+      <c r="G75" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="H75" s="3" t="s">
+        <v>244</v>
+      </c>
+      <c r="J75" s="3" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2492,7 +3525,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="77" spans="1:5" hidden="1" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:10" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2509,7 +3542,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2525,8 +3558,20 @@
       <c r="E78" t="s">
         <v>156</v>
       </c>
-    </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F78" t="s">
+        <v>188</v>
+      </c>
+      <c r="G78" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="H78" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="J78" s="3" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2542,8 +3587,20 @@
       <c r="E79" t="s">
         <v>178</v>
       </c>
-    </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F79" t="s">
+        <v>188</v>
+      </c>
+      <c r="G79" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="H79" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="J79" s="6">
+        <v>88978980784.304398</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2559,8 +3616,20 @@
       <c r="E80" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F80" t="s">
+        <v>188</v>
+      </c>
+      <c r="G80" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="H80" s="3" t="s">
+        <v>243</v>
+      </c>
+      <c r="J80" s="3" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2576,8 +3645,20 @@
       <c r="E81" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F81" t="s">
+        <v>188</v>
+      </c>
+      <c r="G81" s="3" t="s">
+        <v>277</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="J81" s="6">
+        <v>222070211748.35901</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2593,8 +3674,20 @@
       <c r="E82" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F82" t="s">
+        <v>188</v>
+      </c>
+      <c r="G82" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="H82" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="J82" s="3" t="s">
+        <v>326</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2610,8 +3703,20 @@
       <c r="E83" t="s">
         <v>171</v>
       </c>
-    </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F83" t="s">
+        <v>188</v>
+      </c>
+      <c r="G83" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="H83" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="J83" s="3" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2627,8 +3732,20 @@
       <c r="E84" t="s">
         <v>182</v>
       </c>
-    </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F84" t="s">
+        <v>188</v>
+      </c>
+      <c r="G84" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="H84" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="J84" s="3" t="s">
+        <v>329</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2644,8 +3761,20 @@
       <c r="E85" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F85" t="s">
+        <v>188</v>
+      </c>
+      <c r="G85" s="3" t="s">
+        <v>251</v>
+      </c>
+      <c r="H85" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="J85" s="3" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="86" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2661,8 +3790,20 @@
       <c r="E86" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F86" t="s">
+        <v>188</v>
+      </c>
+      <c r="G86" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="H86" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="J86" s="3" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="87" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2678,8 +3819,20 @@
       <c r="E87" t="s">
         <v>183</v>
       </c>
-    </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F87" t="s">
+        <v>188</v>
+      </c>
+      <c r="G87" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="H87" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="J87" s="3" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="88" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -2695,8 +3848,20 @@
       <c r="E88" t="s">
         <v>150</v>
       </c>
-    </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F88" t="s">
+        <v>188</v>
+      </c>
+      <c r="G88" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="H88" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="J88" s="3" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="89" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -2712,8 +3877,20 @@
       <c r="E89" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="F89" t="s">
+        <v>188</v>
+      </c>
+      <c r="G89" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="H89" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="J89" s="3" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="90" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -2730,7 +3907,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -2747,7 +3924,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -2764,7 +3941,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -2781,7 +3958,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -2798,7 +3975,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -2815,7 +3992,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:10" x14ac:dyDescent="0.35">
       <c r="A96" s="1">
         <v>94</v>
       </c>

</xml_diff>